<commit_message>
fix bugs in program
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,74 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>drop the kids in school</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-11-18</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>kids holiday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-06-28</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dinner with friends</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-08-13</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>school holidays</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-07-12</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>